<commit_message>
add stadium and club info to db and add to club view
</commit_message>
<xml_diff>
--- a/FTW feature list.xlsx
+++ b/FTW feature list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andypierce/Desktop/ftw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8BAAEF1-957A-D448-99FE-150FF6E88DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51F3FE0C-CD14-E641-9BB4-3ACB18BAAC4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30240" yWindow="-8660" windowWidth="51200" windowHeight="28300" xr2:uid="{F7CEB26F-511F-304C-8A6C-3D3E353055BD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="70">
   <si>
     <t>Match</t>
   </si>
@@ -62,9 +62,6 @@
     <t>list a player</t>
   </si>
   <si>
-    <t>stadium</t>
-  </si>
-  <si>
     <t>commentary</t>
   </si>
   <si>
@@ -89,15 +86,6 @@
     <t>cards</t>
   </si>
   <si>
-    <t>hidden stats</t>
-  </si>
-  <si>
-    <t>note: things like tactics directly affect the team totals calc</t>
-  </si>
-  <si>
-    <t>note: things like hidden stats affect player match perf calcs</t>
-  </si>
-  <si>
     <t xml:space="preserve">sponsorship </t>
   </si>
   <si>
@@ -110,12 +98,6 @@
     <t>Admin</t>
   </si>
   <si>
-    <t>front end for user</t>
-  </si>
-  <si>
-    <t>user login</t>
-  </si>
-  <si>
     <t>special events like community chance in monopoly</t>
   </si>
   <si>
@@ -137,7 +119,133 @@
     <t>substitutions</t>
   </si>
   <si>
-    <t>turn output</t>
+    <t>potential</t>
+  </si>
+  <si>
+    <t>star stat</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>blend</t>
+  </si>
+  <si>
+    <t>home advantage</t>
+  </si>
+  <si>
+    <t>contracts</t>
+  </si>
+  <si>
+    <t>Post playtest</t>
+  </si>
+  <si>
+    <t>Pre playtest</t>
+  </si>
+  <si>
+    <t>users</t>
+  </si>
+  <si>
+    <t>player turn view</t>
+  </si>
+  <si>
+    <t>player turn entry</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>board interactions</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>club creation</t>
+  </si>
+  <si>
+    <t>Pre launch</t>
+  </si>
+  <si>
+    <t>payment system</t>
+  </si>
+  <si>
+    <t>player emails/comms</t>
+  </si>
+  <si>
+    <t>deployment</t>
+  </si>
+  <si>
+    <t>stadium &amp; club</t>
+  </si>
+  <si>
+    <t>n s e w stands with names</t>
+  </si>
+  <si>
+    <t>ground name</t>
+  </si>
+  <si>
+    <t>boxes</t>
+  </si>
+  <si>
+    <t>facility level linked to attendance</t>
+  </si>
+  <si>
+    <t>condition linked to attendance</t>
+  </si>
+  <si>
+    <t>fan loyalty</t>
+  </si>
+  <si>
+    <t>things to add:</t>
+  </si>
+  <si>
+    <t>capability to improve - system to upgrade.  Unlimited seating capacity</t>
+  </si>
+  <si>
+    <t>club colours</t>
+  </si>
+  <si>
+    <t>can improve</t>
+  </si>
+  <si>
+    <t>Fixtures</t>
+  </si>
+  <si>
+    <t>edit</t>
+  </si>
+  <si>
+    <t>cup comps</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>international management</t>
+  </si>
+  <si>
+    <t>manager rating</t>
+  </si>
+  <si>
+    <t>dfc</t>
+  </si>
+  <si>
+    <t>mid</t>
+  </si>
+  <si>
+    <t>att</t>
+  </si>
+  <si>
+    <t>gkp</t>
+  </si>
+  <si>
+    <t>scout dept</t>
   </si>
 </sst>
 </file>
@@ -154,7 +262,7 @@
     </font>
     <font>
       <b/>
-      <sz val="20"/>
+      <sz val="24"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -162,15 +270,15 @@
     </font>
     <font>
       <b/>
-      <sz val="14"/>
-      <color theme="1"/>
+      <sz val="12"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="24"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -186,7 +294,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -203,22 +311,43 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -534,140 +663,454 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83BAFEFB-A687-D349-960B-4C897E7814D4}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:V44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="6" width="31.1640625" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="12.5" style="3" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57.83203125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="11"/>
+    <col min="5" max="5" width="13.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="10.83203125" style="9"/>
+    <col min="12" max="22" width="10.83203125" style="11"/>
+    <col min="23" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="64" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:12" ht="31" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="9"/>
+    </row>
+    <row r="3" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="6"/>
+      <c r="B5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="6"/>
+      <c r="B6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="6"/>
+      <c r="B7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="6"/>
+      <c r="B8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="6"/>
+      <c r="B9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="6"/>
+      <c r="B10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="6"/>
+      <c r="B11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="6"/>
+      <c r="B12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="6"/>
+      <c r="B13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="L13" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="6"/>
+      <c r="B14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="6"/>
+      <c r="B15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="6"/>
+      <c r="B16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" ht="27" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="6"/>
+      <c r="B17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="6"/>
+      <c r="B18" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="6"/>
+      <c r="B19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="6"/>
+      <c r="B20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="6"/>
+      <c r="B21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="6"/>
+      <c r="B22" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="6"/>
+    </row>
+    <row r="24" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="6"/>
+      <c r="B25" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="6"/>
+      <c r="B26" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="6"/>
+      <c r="B27" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="6"/>
+      <c r="B28" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B29" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B30" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B31" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C31" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B32" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C32" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B33" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="C33" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="2" t="s">
+    </row>
+    <row r="34" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B34" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="2" t="s">
+    </row>
+    <row r="35" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B35" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>32</v>
+    </row>
+    <row r="36" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B36" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B37" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B38" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B39" s="2"/>
+      <c r="C39" s="1"/>
+    </row>
+    <row r="40" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B41" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B42" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B43" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="B44" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some error messaging implimented
</commit_message>
<xml_diff>
--- a/FTW feature list.xlsx
+++ b/FTW feature list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andypierce/Desktop/ftw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A14787-1346-DD41-BEA1-EC07D112A1A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D558054E-3BC5-9646-9A29-1EA9070CBCD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{F7CEB26F-511F-304C-8A6C-3D3E353055BD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="65">
   <si>
     <t>Match</t>
   </si>
@@ -228,6 +228,9 @@
   </si>
   <si>
     <t>initial form for working elements, team selection, training, upgrades.  JS validation</t>
+  </si>
+  <si>
+    <t>pundit gem</t>
   </si>
 </sst>
 </file>
@@ -274,7 +277,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -299,12 +302,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -318,7 +315,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -357,9 +354,6 @@
       <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -681,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83BAFEFB-A687-D349-960B-4C897E7814D4}">
   <dimension ref="A1:W42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -777,7 +771,7 @@
         <v>49</v>
       </c>
       <c r="E4" s="13"/>
-      <c r="H4" s="15" t="s">
+      <c r="H4" s="14" t="s">
         <v>53</v>
       </c>
       <c r="M4" s="3" t="s">
@@ -796,7 +790,7 @@
         <v>50</v>
       </c>
       <c r="E5" s="13"/>
-      <c r="H5" s="15"/>
+      <c r="H5" s="14"/>
       <c r="M5" s="3" t="s">
         <v>54</v>
       </c>
@@ -810,7 +804,7 @@
         <v>25</v>
       </c>
       <c r="E6" s="13"/>
-      <c r="H6" s="15"/>
+      <c r="H6" s="14"/>
       <c r="M6" s="3" t="s">
         <v>55</v>
       </c>
@@ -827,7 +821,7 @@
         <v>12</v>
       </c>
       <c r="E7" s="13"/>
-      <c r="H7" s="15"/>
+      <c r="H7" s="14"/>
       <c r="M7" s="3" t="s">
         <v>54</v>
       </c>
@@ -844,7 +838,7 @@
         <v>50</v>
       </c>
       <c r="E8" s="13"/>
-      <c r="H8" s="15"/>
+      <c r="H8" s="14"/>
       <c r="M8" s="3" t="s">
         <v>54</v>
       </c>
@@ -857,8 +851,8 @@
       <c r="D9" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E9" s="14"/>
-      <c r="H9" s="15"/>
+      <c r="E9" s="13"/>
+      <c r="H9" s="14"/>
       <c r="M9" s="3" t="s">
         <v>63</v>
       </c>
@@ -866,42 +860,45 @@
     <row r="10" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="3" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="1"/>
+        <v>30</v>
+      </c>
       <c r="F10" s="11"/>
-      <c r="H10" s="15"/>
-      <c r="M10" s="3"/>
+      <c r="H10" s="14"/>
+      <c r="M10" s="3" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="11" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>60</v>
+        <v>8</v>
       </c>
       <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
       <c r="G11" s="11"/>
-      <c r="H11" s="15"/>
-      <c r="M11" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="H11" s="14"/>
+      <c r="M11" s="3"/>
     </row>
     <row r="12" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="3" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>9</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="E12" s="1"/>
       <c r="G12" s="11"/>
-      <c r="H12" s="15"/>
-      <c r="M12" s="3"/>
+      <c r="H12" s="14"/>
+      <c r="M12" s="3" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="13" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
@@ -909,22 +906,22 @@
         <v>0</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H13" s="15"/>
-      <c r="I13" s="12"/>
+        <v>9</v>
+      </c>
+      <c r="G13" s="11"/>
+      <c r="H13" s="14"/>
       <c r="M13" s="3"/>
     </row>
     <row r="14" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H14" s="15"/>
-      <c r="J14" s="12"/>
+        <v>10</v>
+      </c>
+      <c r="H14" s="14"/>
+      <c r="I14" s="12"/>
       <c r="M14" s="3"/>
     </row>
     <row r="15" spans="1:23" ht="17" x14ac:dyDescent="0.2">
@@ -933,14 +930,11 @@
         <v>3</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G15" s="1"/>
-      <c r="H15" s="15"/>
-      <c r="K15" s="12"/>
-      <c r="M15" s="3" t="s">
-        <v>59</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="H15" s="14"/>
+      <c r="J15" s="12"/>
+      <c r="M15" s="3"/>
     </row>
     <row r="16" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
@@ -948,12 +942,13 @@
         <v>3</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H16" s="15"/>
+        <v>26</v>
+      </c>
+      <c r="G16" s="1"/>
+      <c r="H16" s="14"/>
       <c r="K16" s="12"/>
       <c r="M16" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -962,25 +957,27 @@
         <v>3</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H17" s="15"/>
-      <c r="L17" s="12"/>
+        <v>51</v>
+      </c>
+      <c r="H17" s="14"/>
+      <c r="K17" s="12"/>
       <c r="M17" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="3" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H18" s="15"/>
+        <v>27</v>
+      </c>
+      <c r="H18" s="14"/>
       <c r="L18" s="12"/>
-      <c r="M18" s="3"/>
+      <c r="M18" s="3" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="19" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
@@ -990,7 +987,7 @@
       <c r="D19" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H19" s="15"/>
+      <c r="H19" s="14"/>
       <c r="L19" s="12"/>
       <c r="M19" s="3"/>
     </row>
@@ -1002,13 +999,13 @@
       <c r="D20" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H20" s="15"/>
+      <c r="H20" s="14"/>
       <c r="L20" s="12"/>
       <c r="M20" s="3"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
-      <c r="H21" s="15"/>
+      <c r="H21" s="14"/>
       <c r="M21" s="3"/>
     </row>
     <row r="22" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -1021,7 +1018,7 @@
       <c r="D22" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H22" s="15"/>
+      <c r="H22" s="14"/>
       <c r="M22" s="3"/>
     </row>
     <row r="23" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -1032,7 +1029,7 @@
       <c r="D23" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H23" s="15"/>
+      <c r="H23" s="14"/>
       <c r="M23" s="3"/>
     </row>
     <row r="24" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -1043,7 +1040,7 @@
       <c r="D24" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H24" s="15"/>
+      <c r="H24" s="14"/>
       <c r="M24" s="3"/>
     </row>
     <row r="25" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -1054,7 +1051,7 @@
       <c r="D25" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H25" s="15"/>
+      <c r="H25" s="14"/>
       <c r="M25" s="3"/>
     </row>
     <row r="26" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -1064,7 +1061,7 @@
       <c r="D26" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H26" s="15"/>
+      <c r="H26" s="14"/>
       <c r="M26" s="3"/>
     </row>
     <row r="27" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -1074,7 +1071,7 @@
       <c r="D27" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H27" s="15"/>
+      <c r="H27" s="14"/>
       <c r="M27" s="3"/>
     </row>
     <row r="28" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -1084,7 +1081,7 @@
       <c r="D28" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H28" s="15"/>
+      <c r="H28" s="14"/>
       <c r="M28" s="3"/>
     </row>
     <row r="29" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -1094,7 +1091,7 @@
       <c r="D29" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H29" s="15"/>
+      <c r="H29" s="14"/>
       <c r="M29" s="3"/>
     </row>
     <row r="30" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -1104,7 +1101,7 @@
       <c r="D30" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H30" s="15"/>
+      <c r="H30" s="14"/>
       <c r="M30" s="3"/>
     </row>
     <row r="31" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -1114,7 +1111,7 @@
       <c r="D31" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H31" s="15"/>
+      <c r="H31" s="14"/>
       <c r="M31" s="3"/>
     </row>
     <row r="32" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -1124,7 +1121,7 @@
       <c r="D32" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H32" s="15"/>
+      <c r="H32" s="14"/>
       <c r="M32" s="3"/>
     </row>
     <row r="33" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -1134,7 +1131,7 @@
       <c r="D33" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="H33" s="15"/>
+      <c r="H33" s="14"/>
       <c r="M33" s="3"/>
     </row>
     <row r="34" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -1144,7 +1141,7 @@
       <c r="D34" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="H34" s="15"/>
+      <c r="H34" s="14"/>
       <c r="M34" s="3"/>
     </row>
     <row r="35" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -1154,14 +1151,14 @@
       <c r="D35" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="H35" s="15"/>
+      <c r="H35" s="14"/>
       <c r="M35" s="3"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
-      <c r="H36" s="15"/>
+      <c r="H36" s="14"/>
       <c r="M36" s="3"/>
     </row>
     <row r="37" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -1174,7 +1171,7 @@
       <c r="D37" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H37" s="15"/>
+      <c r="H37" s="14"/>
       <c r="M37" s="3"/>
     </row>
     <row r="38" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -1184,7 +1181,7 @@
       <c r="D38" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H38" s="15"/>
+      <c r="H38" s="14"/>
       <c r="M38" s="3"/>
     </row>
     <row r="39" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -1194,7 +1191,7 @@
       <c r="D39" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H39" s="15"/>
+      <c r="H39" s="14"/>
       <c r="M39" s="3"/>
     </row>
     <row r="40" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -1204,7 +1201,7 @@
       <c r="D40" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H40" s="15"/>
+      <c r="H40" s="14"/>
       <c r="M40" s="3"/>
     </row>
     <row r="41" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -1214,7 +1211,7 @@
       <c r="D41" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="H41" s="15"/>
+      <c r="H41" s="14"/>
       <c r="M41" s="3"/>
     </row>
     <row r="42" spans="1:13" ht="17" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
match commentary functionality fully working
</commit_message>
<xml_diff>
--- a/FTW feature list.xlsx
+++ b/FTW feature list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andypierce/Desktop/ftw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D558054E-3BC5-9646-9A29-1EA9070CBCD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A4431FA-5E7E-A544-BFDB-CC2D2FBD2AF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{F7CEB26F-511F-304C-8A6C-3D3E353055BD}"/>
   </bookViews>
@@ -230,7 +230,7 @@
     <t>initial form for working elements, team selection, training, upgrades.  JS validation</t>
   </si>
   <si>
-    <t>pundit gem</t>
+    <t>need to enhance comments</t>
   </si>
 </sst>
 </file>
@@ -675,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83BAFEFB-A687-D349-960B-4C897E7814D4}">
   <dimension ref="A1:W42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -867,9 +867,7 @@
       </c>
       <c r="F10" s="11"/>
       <c r="H10" s="14"/>
-      <c r="M10" s="3" t="s">
-        <v>64</v>
-      </c>
+      <c r="M10" s="3"/>
     </row>
     <row r="11" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
@@ -880,10 +878,11 @@
         <v>8</v>
       </c>
       <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="11"/>
+      <c r="F11" s="13"/>
       <c r="H11" s="14"/>
-      <c r="M11" s="3"/>
+      <c r="M11" s="3" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="12" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>

</xml_diff>

<commit_message>
tactics working but no views yet
</commit_message>
<xml_diff>
--- a/FTW feature list.xlsx
+++ b/FTW feature list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andypierce/Desktop/ftw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C7BE14-3F45-0244-BD54-813D3F7AD755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A07B97-8E10-1542-8169-40002CCC29F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{F7CEB26F-511F-304C-8A6C-3D3E353055BD}"/>
+    <workbookView xWindow="-36420" yWindow="-160" windowWidth="30240" windowHeight="18880" xr2:uid="{F7CEB26F-511F-304C-8A6C-3D3E353055BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="66">
   <si>
     <t>Match</t>
   </si>
@@ -231,6 +231,9 @@
   </si>
   <si>
     <t>add more commentary examples and rewrite existing ones</t>
+  </si>
+  <si>
+    <t>data management</t>
   </si>
 </sst>
 </file>
@@ -673,10 +676,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83BAFEFB-A687-D349-960B-4C897E7814D4}">
-  <dimension ref="A1:W43"/>
+  <dimension ref="A1:W44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -872,42 +875,42 @@
     <row r="11" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="3" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="13"/>
+        <v>65</v>
+      </c>
+      <c r="F11" s="11"/>
       <c r="H11" s="14"/>
       <c r="M11" s="3"/>
     </row>
     <row r="12" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="E12" s="1"/>
-      <c r="G12" s="11"/>
+      <c r="F12" s="13"/>
       <c r="H12" s="14"/>
-      <c r="M12" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="M12" s="3"/>
     </row>
     <row r="13" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="3" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>8</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="E13" s="1"/>
       <c r="G13" s="11"/>
       <c r="H13" s="14"/>
-      <c r="M13" s="3"/>
+      <c r="M13" s="3" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="14" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
@@ -915,19 +918,19 @@
         <v>0</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>9</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="G14" s="11"/>
       <c r="H14" s="14"/>
-      <c r="I14" s="12"/>
       <c r="M14" s="3"/>
     </row>
     <row r="15" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H15" s="14"/>
       <c r="I15" s="12"/>
@@ -939,14 +942,11 @@
         <v>3</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G16" s="1"/>
+        <v>12</v>
+      </c>
       <c r="H16" s="14"/>
-      <c r="J16" s="12"/>
-      <c r="M16" s="3" t="s">
-        <v>58</v>
-      </c>
+      <c r="I16" s="12"/>
+      <c r="M16" s="3"/>
     </row>
     <row r="17" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
@@ -954,12 +954,13 @@
         <v>3</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>50</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="G17" s="1"/>
       <c r="H17" s="14"/>
       <c r="J17" s="12"/>
       <c r="M17" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -968,12 +969,12 @@
         <v>3</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="H18" s="14"/>
-      <c r="K18" s="12"/>
+      <c r="J18" s="12"/>
       <c r="M18" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -982,62 +983,65 @@
         <v>3</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="H19" s="14"/>
       <c r="K19" s="12"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="3"/>
+      <c r="M19" s="3" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="20" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="3" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="H20" s="14"/>
-      <c r="L20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="1"/>
       <c r="M20" s="3"/>
     </row>
     <row r="21" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" s="3" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="H21" s="14"/>
       <c r="L21" s="12"/>
       <c r="M21" s="3"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
+      <c r="B22" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="H22" s="14"/>
+      <c r="L22" s="12"/>
       <c r="M22" s="3"/>
     </row>
-    <row r="23" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>17</v>
-      </c>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" s="4"/>
       <c r="H23" s="14"/>
       <c r="M23" s="3"/>
     </row>
     <row r="24" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="4"/>
+      <c r="A24" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="B24" s="3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="H24" s="14"/>
       <c r="M24" s="3"/>
@@ -1048,7 +1052,7 @@
         <v>4</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H25" s="14"/>
       <c r="M25" s="3"/>
@@ -1059,17 +1063,18 @@
         <v>4</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="H26" s="14"/>
       <c r="M26" s="3"/>
     </row>
     <row r="27" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="4"/>
       <c r="B27" s="3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H27" s="14"/>
       <c r="M27" s="3"/>
@@ -1079,47 +1084,47 @@
         <v>2</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H28" s="14"/>
       <c r="M28" s="3"/>
     </row>
     <row r="29" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B29" s="3" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H29" s="14"/>
       <c r="M29" s="3"/>
     </row>
     <row r="30" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B30" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H30" s="14"/>
       <c r="M30" s="3"/>
     </row>
     <row r="31" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B31" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="H31" s="14"/>
       <c r="M31" s="3"/>
     </row>
     <row r="32" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B32" s="3" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="H32" s="14"/>
       <c r="M32" s="3"/>
@@ -1129,27 +1134,27 @@
         <v>0</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="H33" s="14"/>
       <c r="M33" s="3"/>
     </row>
     <row r="34" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B34" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="H34" s="14"/>
       <c r="M34" s="3"/>
     </row>
     <row r="35" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B35" s="3" t="s">
-        <v>39</v>
+        <v>1</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="H35" s="14"/>
       <c r="M35" s="3"/>
@@ -1159,37 +1164,37 @@
         <v>39</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H36" s="14"/>
       <c r="M36" s="3"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
+    <row r="37" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="B37" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="H37" s="14"/>
       <c r="M37" s="3"/>
     </row>
-    <row r="38" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>34</v>
-      </c>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
       <c r="H38" s="14"/>
       <c r="M38" s="3"/>
     </row>
     <row r="39" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="B39" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H39" s="14"/>
       <c r="M39" s="3"/>
@@ -1199,17 +1204,17 @@
         <v>33</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H40" s="14"/>
       <c r="M40" s="3"/>
     </row>
     <row r="41" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B41" s="3" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="H41" s="14"/>
       <c r="M41" s="3"/>
@@ -1219,22 +1224,32 @@
         <v>42</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H42" s="14"/>
       <c r="M42" s="3"/>
     </row>
     <row r="43" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B43" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H43" s="14"/>
+      <c r="M43" s="3"/>
+    </row>
+    <row r="44" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="B44" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D44" s="3" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="H4:H42"/>
+    <mergeCell ref="H4:H43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
seed files for game creation completed
</commit_message>
<xml_diff>
--- a/FTW feature list.xlsx
+++ b/FTW feature list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andypierce/Desktop/ftw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE880CED-482D-784B-8A4F-99F354823F22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C55A29-52F8-8D4A-AEA5-BFE0B7FB350D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{F7CEB26F-511F-304C-8A6C-3D3E353055BD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="67">
   <si>
     <t>Match</t>
   </si>
@@ -234,6 +234,9 @@
   </si>
   <si>
     <t>data management</t>
+  </si>
+  <si>
+    <t>fixture list, club names, club abbr, players by position with potential</t>
   </si>
 </sst>
 </file>
@@ -676,10 +679,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83BAFEFB-A687-D349-960B-4C897E7814D4}">
-  <dimension ref="A1:W44"/>
+  <dimension ref="A1:W45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:F11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -868,7 +871,7 @@
       <c r="D10" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
       <c r="H10" s="14"/>
       <c r="M10" s="3"/>
     </row>
@@ -880,49 +883,53 @@
       <c r="D11" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
       <c r="H11" s="14"/>
       <c r="M11" s="3"/>
     </row>
     <row r="12" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="3" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="13"/>
+        <v>51</v>
+      </c>
+      <c r="G12" s="11"/>
       <c r="H12" s="14"/>
-      <c r="M12" s="3"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="3" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="13" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="E13" s="1"/>
-      <c r="G13" s="13"/>
+      <c r="F13" s="13"/>
       <c r="H13" s="14"/>
-      <c r="M13" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="M13" s="3"/>
     </row>
     <row r="14" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="3" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G14" s="13"/>
+        <v>59</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="1"/>
       <c r="H14" s="14"/>
-      <c r="M14" s="3"/>
+      <c r="M14" s="3" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="15" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
@@ -930,19 +937,20 @@
         <v>0</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>9</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="F15" s="13"/>
+      <c r="G15" s="1"/>
       <c r="H15" s="14"/>
-      <c r="I15" s="12"/>
       <c r="M15" s="3"/>
     </row>
     <row r="16" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H16" s="14"/>
       <c r="I16" s="12"/>
@@ -954,14 +962,11 @@
         <v>3</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G17" s="1"/>
+        <v>12</v>
+      </c>
       <c r="H17" s="14"/>
-      <c r="J17" s="12"/>
-      <c r="M17" s="3" t="s">
-        <v>58</v>
-      </c>
+      <c r="I17" s="12"/>
+      <c r="M17" s="3"/>
     </row>
     <row r="18" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
@@ -969,12 +974,13 @@
         <v>3</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>50</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="G18" s="1"/>
       <c r="H18" s="14"/>
       <c r="J18" s="12"/>
       <c r="M18" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -983,12 +989,12 @@
         <v>3</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="H19" s="14"/>
-      <c r="K19" s="12"/>
+      <c r="J19" s="12"/>
       <c r="M19" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -997,62 +1003,65 @@
         <v>3</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="H20" s="14"/>
       <c r="K20" s="12"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="3"/>
+      <c r="M20" s="3" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="21" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" s="3" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="H21" s="14"/>
-      <c r="L21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="1"/>
       <c r="M21" s="3"/>
     </row>
     <row r="22" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
       <c r="B22" s="3" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="H22" s="14"/>
       <c r="L22" s="12"/>
       <c r="M22" s="3"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
+      <c r="B23" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="H23" s="14"/>
+      <c r="L23" s="12"/>
       <c r="M23" s="3"/>
     </row>
-    <row r="24" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>17</v>
-      </c>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24" s="4"/>
       <c r="H24" s="14"/>
       <c r="M24" s="3"/>
     </row>
     <row r="25" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="4"/>
+      <c r="A25" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="B25" s="3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="H25" s="14"/>
       <c r="M25" s="3"/>
@@ -1063,7 +1072,7 @@
         <v>4</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H26" s="14"/>
       <c r="M26" s="3"/>
@@ -1074,17 +1083,18 @@
         <v>4</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="H27" s="14"/>
       <c r="M27" s="3"/>
     </row>
     <row r="28" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="4"/>
       <c r="B28" s="3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H28" s="14"/>
       <c r="M28" s="3"/>
@@ -1094,47 +1104,47 @@
         <v>2</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H29" s="14"/>
       <c r="M29" s="3"/>
     </row>
     <row r="30" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B30" s="3" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H30" s="14"/>
       <c r="M30" s="3"/>
     </row>
     <row r="31" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B31" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H31" s="14"/>
       <c r="M31" s="3"/>
     </row>
     <row r="32" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B32" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="H32" s="14"/>
       <c r="M32" s="3"/>
     </row>
     <row r="33" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B33" s="3" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="H33" s="14"/>
       <c r="M33" s="3"/>
@@ -1144,27 +1154,27 @@
         <v>0</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="H34" s="14"/>
       <c r="M34" s="3"/>
     </row>
     <row r="35" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B35" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="H35" s="14"/>
       <c r="M35" s="3"/>
     </row>
     <row r="36" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B36" s="3" t="s">
-        <v>39</v>
+        <v>1</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="H36" s="14"/>
       <c r="M36" s="3"/>
@@ -1174,37 +1184,37 @@
         <v>39</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H37" s="14"/>
       <c r="M37" s="3"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
+    <row r="38" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="B38" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="H38" s="14"/>
       <c r="M38" s="3"/>
     </row>
-    <row r="39" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>34</v>
-      </c>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
       <c r="H39" s="14"/>
       <c r="M39" s="3"/>
     </row>
     <row r="40" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="B40" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H40" s="14"/>
       <c r="M40" s="3"/>
@@ -1214,17 +1224,17 @@
         <v>33</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H41" s="14"/>
       <c r="M41" s="3"/>
     </row>
     <row r="42" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B42" s="3" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="H42" s="14"/>
       <c r="M42" s="3"/>
@@ -1234,22 +1244,32 @@
         <v>42</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H43" s="14"/>
       <c r="M43" s="3"/>
     </row>
     <row r="44" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B44" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H44" s="14"/>
+      <c r="M44" s="3"/>
+    </row>
+    <row r="45" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="B45" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="D45" s="3" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="H4:H43"/>
+    <mergeCell ref="H4:H44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>